<commit_message>
Added functional grey box tests to doc
</commit_message>
<xml_diff>
--- a/GreyBoxTesting.xlsx
+++ b/GreyBoxTesting.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
   <si>
     <t xml:space="preserve">GREY BOX TESTING</t>
   </si>
@@ -95,6 +95,39 @@
   </si>
   <si>
     <t xml:space="preserve">TC_GBT_06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">League Create Method adds a new object to the database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_GBT_07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">League object with the Year set to “2007”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Database has one more item in it than it did previously</t>
+  </si>
+  <si>
+    <t xml:space="preserve">League Edit Method updates an object in the database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_GBT_08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 and League object with Year set to “2019”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Database now has a league object that has the Year set to “2019”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">League Delete Method deletes an object from the database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_GBT_09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Database has one less item in it than it did previousy</t>
   </si>
 </sst>
 </file>
@@ -396,8 +429,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -555,6 +588,68 @@
         <v>12</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Finished grey box doc
</commit_message>
<xml_diff>
--- a/GreyBoxTesting.xlsx
+++ b/GreyBoxTesting.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="80">
   <si>
     <t xml:space="preserve">GREY BOX TESTING</t>
   </si>
@@ -67,7 +67,7 @@
     <t xml:space="preserve">TC_GBT_02</t>
   </si>
   <si>
-    <t xml:space="preserve">LeaguesController</t>
+    <t xml:space="preserve">LeagueController</t>
   </si>
   <si>
     <t xml:space="preserve">Database Context</t>
@@ -128,6 +128,138 @@
   </si>
   <si>
     <t xml:space="preserve">The Database has one less item in it than it did previousy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Index Page in Match Controller returns a valid response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_GBT_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MatchController</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Details Page in Match Controller returns a valid response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_GBT_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Page in Match Controller returns a valid response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_GBT_12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit Page in Match Controller returns a valid response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_GBT_13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete Page in Match Controller returns a valid response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_GBT_14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Index Page in Player Controller returns a valid response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_GBT_15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PlayerController</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Details Page in Player Controller returns a valid response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_GBT_16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Page in Player Controller returns a valid response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_GBT_17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit Page in Player Controller returns a valid response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_GBT_18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete Page in Player Controller returns a valid response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_GBT_19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Index Page in Stats Controller returns a valid response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_GBT_20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StatsController</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Details Page in Stats Controller returns a valid response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_GBT_21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Page in Stats Controller returns a valid response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_GBT_22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit Page in Stats Controller returns a valid response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_GBT_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete Page in Stats Controller returns a valid response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_GBT_24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Index Page in Team Controller returns a valid response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_GBT_25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TeamController</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Details Page in Team Controller returns a valid response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_GBT_26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Page in Team Controller returns a valid response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_GBT_27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit Page in Team Controller returns a valid response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_GBT_28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete Page in Team Controller returns a valid response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_GBT_29</t>
   </si>
 </sst>
 </file>
@@ -429,8 +561,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -648,8 +780,406 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>